<commit_message>
fix empty unknown_column_name list warning
</commit_message>
<xml_diff>
--- a/input/xiaobai1.xlsx
+++ b/input/xiaobai1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bytedance/PycharmProjects/pythonProject/order/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bytedance/PycharmProjects/order/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B53B80-7E87-9E46-BD38-0C2F971061A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9B0D8B-B14F-FA4E-880F-0376D200FCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,34 +117,6 @@
   </si>
   <si>
     <t>20250220100542bajgdnx</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="15"/>
-        <color rgb="FF000000"/>
-        <rFont val="Microsoft YaHei"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">  订单编号</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="15"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 物流公司  </t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>斯亚旦发皂三块装</t>
@@ -186,12 +158,20 @@
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>订单编号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>物流公司</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -222,14 +202,6 @@
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Microsoft YaHei"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
     </font>
@@ -274,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -291,13 +263,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -607,7 +576,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -625,11 +594,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22">
-      <c r="A1" s="5" t="s">
-        <v>28</v>
+      <c r="A1" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -699,7 +668,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>13</v>
@@ -724,8 +693,8 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>31</v>
+      <c r="H4" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>13</v>
@@ -750,8 +719,8 @@
       <c r="G5" s="1">
         <v>2</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>32</v>
+      <c r="H5" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>13</v>
@@ -799,7 +768,7 @@
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>4</v>
       </c>
       <c r="H7" s="1" t="s">

</xml_diff>